<commit_message>
Reduced 'Rank' sheet to one row
</commit_message>
<xml_diff>
--- a/2017 Template.xlsx
+++ b/2017 Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaitoarai/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaitoarai/Git/FMS-Scout-2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Match Data" sheetId="1" r:id="rId1"/>
@@ -968,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1705,11 +1705,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U38" sqref="U38"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1914,2274 +1914,566 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B4)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B4)</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!$AA$3:$AA$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AC$3:AC$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AD$3:AD$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AE$3:AE$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AF$3:AF$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AG$3:AG$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AH$3:AH$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AI$3:AI$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AJ$3:AJ$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AK$3:AK$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AL$3:AL$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AM$3:AM$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AN$3:AN$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AO$3:AO$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AP$3:AP$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AQ$3:AQ$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AR$3:AR$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U4" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B4,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B4,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B4,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B4,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B4,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B4,'Raw Match Data'!AS$3:AS$128))/(3*$C4)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B5)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B5)</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!$AA$3:$AA$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AC$3:AC$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AD$3:AD$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AE$3:AE$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AF$3:AF$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AG$3:AG$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AH$3:AH$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AI$3:AI$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AJ$3:AJ$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AK$3:AK$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AL$3:AL$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AM$3:AM$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AN$3:AN$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AO$3:AO$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AP$3:AP$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AQ$3:AQ$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AR$3:AR$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U5" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B5,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B5,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B5,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B5,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B5,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B5,'Raw Match Data'!AS$3:AS$128))/(3*$C5)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B6)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B6)</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!$AA$3:$AA$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AC$3:AC$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AD$3:AD$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AE$3:AE$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AF$3:AF$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AG$3:AG$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AH$3:AH$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AI$3:AI$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AJ$3:AJ$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AK$3:AK$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AL$3:AL$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AM$3:AM$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AN$3:AN$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AO$3:AO$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AP$3:AP$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AQ$3:AQ$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AR$3:AR$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B6,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B6,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B6,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B6,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B6,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B6,'Raw Match Data'!AS$3:AS$128))/(3*$C6)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B7)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B7)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!$AA$3:$AA$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AC$3:AC$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AD$3:AD$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AE$3:AE$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AF$3:AF$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AG$3:AG$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AH$3:AH$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AI$3:AI$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AJ$3:AJ$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AK$3:AK$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AL$3:AL$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AM$3:AM$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AN$3:AN$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AO$3:AO$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AP$3:AP$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AQ$3:AQ$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AR$3:AR$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U7" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B7,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B7,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B7,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B7,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B7,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B7,'Raw Match Data'!AS$3:AS$128))/(3*$C7)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B8)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B8)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!$AA$3:$AA$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AC$3:AC$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AD$3:AD$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AE$3:AE$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AF$3:AF$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AG$3:AG$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AH$3:AH$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AI$3:AI$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AJ$3:AJ$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AK$3:AK$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AL$3:AL$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AM$3:AM$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AN$3:AN$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AO$3:AO$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AP$3:AP$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AQ$3:AQ$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AR$3:AR$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U8" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B8,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B8,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B8,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B8,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B8,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B8,'Raw Match Data'!AS$3:AS$128))/(3*$C8)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B9)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B9)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!$AA$3:$AA$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AC$3:AC$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AD$3:AD$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AE$3:AE$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AF$3:AF$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AG$3:AG$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AH$3:AH$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AI$3:AI$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AJ$3:AJ$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AK$3:AK$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AL$3:AL$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AM$3:AM$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AN$3:AN$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AO$3:AO$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AP$3:AP$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AQ$3:AQ$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AR$3:AR$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U9" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B9,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B9,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B9,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B9,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B9,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B9,'Raw Match Data'!AS$3:AS$128))/(3*$C9)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B10)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B10)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!$AA$3:$AA$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AC$3:AC$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AD$3:AD$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AE$3:AE$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AF$3:AF$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AG$3:AG$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AH$3:AH$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AI$3:AI$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AJ$3:AJ$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AK$3:AK$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AL$3:AL$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AM$3:AM$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AN$3:AN$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AO$3:AO$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AP$3:AP$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AQ$3:AQ$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AR$3:AR$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U10" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B10,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B10,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B10,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B10,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B10,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B10,'Raw Match Data'!AS$3:AS$128))/(3*$C10)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B11)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B11)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!$AA$3:$AA$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AC$3:AC$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AD$3:AD$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AE$3:AE$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AF$3:AF$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AG$3:AG$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AH$3:AH$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AI$3:AI$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AJ$3:AJ$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AK$3:AK$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AL$3:AL$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AM$3:AM$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AN$3:AN$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AO$3:AO$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AP$3:AP$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AQ$3:AQ$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AR$3:AR$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U11" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B11,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B11,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B11,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B11,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B11,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B11,'Raw Match Data'!AS$3:AS$128))/(3*$C11)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B12)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B12)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!$AA$3:$AA$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AC$3:AC$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AD$3:AD$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AE$3:AE$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AF$3:AF$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AG$3:AG$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AH$3:AH$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AI$3:AI$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AJ$3:AJ$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AK$3:AK$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AL$3:AL$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AM$3:AM$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AN$3:AN$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AO$3:AO$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AP$3:AP$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AQ$3:AQ$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AR$3:AR$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U12" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B12,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B12,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B12,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B12,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B12,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B12,'Raw Match Data'!AS$3:AS$128))/(3*$C12)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B13)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B13)</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!$AA$3:$AA$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AC$3:AC$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AD$3:AD$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AE$3:AE$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AF$3:AF$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AG$3:AG$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AH$3:AH$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AI$3:AI$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AJ$3:AJ$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AK$3:AK$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AL$3:AL$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AM$3:AM$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AN$3:AN$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AO$3:AO$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AP$3:AP$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AQ$3:AQ$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AR$3:AR$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B13,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B13,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B13,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B13,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B13,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B13,'Raw Match Data'!AS$3:AS$128))/(3*$C13)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C13" s="3"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B14)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B14)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!$AA$3:$AA$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AC$3:AC$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AD$3:AD$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AE$3:AE$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AF$3:AF$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AG$3:AG$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AH$3:AH$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AI$3:AI$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AJ$3:AJ$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AK$3:AK$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AL$3:AL$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AM$3:AM$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AN$3:AN$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AO$3:AO$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AP$3:AP$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AQ$3:AQ$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AR$3:AR$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U14" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B14,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B14,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B14,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B14,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B14,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B14,'Raw Match Data'!AS$3:AS$128))/(3*$C14)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C14" s="3"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B15)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B15)</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!$AA$3:$AA$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AC$3:AC$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AD$3:AD$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AE$3:AE$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AF$3:AF$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AG$3:AG$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AH$3:AH$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AI$3:AI$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AJ$3:AJ$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AK$3:AK$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AL$3:AL$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AM$3:AM$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AN$3:AN$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AO$3:AO$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AP$3:AP$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AQ$3:AQ$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AR$3:AR$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U15" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B15,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B15,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B15,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B15,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B15,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B15,'Raw Match Data'!AS$3:AS$128))/(3*$C15)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C15" s="3"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B16)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B16)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!$AA$3:$AA$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AC$3:AC$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AD$3:AD$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AE$3:AE$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AF$3:AF$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AG$3:AG$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AH$3:AH$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AI$3:AI$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AJ$3:AJ$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AK$3:AK$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AL$3:AL$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AM$3:AM$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AN$3:AN$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AO$3:AO$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AP$3:AP$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AQ$3:AQ$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AR$3:AR$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U16" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B16,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B16,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B16,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B16,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B16,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B16,'Raw Match Data'!AS$3:AS$128))/(3*$C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="C17" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B17)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B17)</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!$AA$3:$AA$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AC$3:AC$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AD$3:AD$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AE$3:AE$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AF$3:AF$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AG$3:AG$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AH$3:AH$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AI$3:AI$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AJ$3:AJ$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AK$3:AK$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AL$3:AL$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AM$3:AM$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AN$3:AN$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AO$3:AO$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AP$3:AP$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AQ$3:AQ$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AR$3:AR$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U17" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B17,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B17,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B17,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B17,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B17,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B17,'Raw Match Data'!AS$3:AS$128))/(3*$C17)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B18)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B18)</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!$AA$3:$AA$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AC$3:AC$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AD$3:AD$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AE$3:AE$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AF$3:AF$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AG$3:AG$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AH$3:AH$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AI$3:AI$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AJ$3:AJ$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AK$3:AK$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AL$3:AL$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AM$3:AM$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AN$3:AN$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AO$3:AO$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AP$3:AP$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AQ$3:AQ$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AR$3:AR$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U18" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B18,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B18,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B18,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B18,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B18,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B18,'Raw Match Data'!AS$3:AS$128))/(3*$C18)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B19)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B19)</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!$AA$3:$AA$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AC$3:AC$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AD$3:AD$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AE$3:AE$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AF$3:AF$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AG$3:AG$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AH$3:AH$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AI$3:AI$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AJ$3:AJ$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AK$3:AK$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AL$3:AL$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AM$3:AM$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AN$3:AN$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AO$3:AO$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AP$3:AP$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AQ$3:AQ$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AR$3:AR$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U19" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B19,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B19,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B19,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B19,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B19,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B19,'Raw Match Data'!AS$3:AS$128))/(3*$C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B20)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B20)</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!$AA$3:$AA$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AC$3:AC$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AD$3:AD$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AE$3:AE$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AF$3:AF$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AG$3:AG$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AH$3:AH$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AI$3:AI$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AJ$3:AJ$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AK$3:AK$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AL$3:AL$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AM$3:AM$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AN$3:AN$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AO$3:AO$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AP$3:AP$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AQ$3:AQ$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AR$3:AR$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U20" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B20,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B20,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B20,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B20,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B20,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B20,'Raw Match Data'!AS$3:AS$128))/(3*$C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="C21" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B21)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B21)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!$AA$3:$AA$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AC$3:AC$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AD$3:AD$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AE$3:AE$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AF$3:AF$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AG$3:AG$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AH$3:AH$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AI$3:AI$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AJ$3:AJ$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AK$3:AK$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AL$3:AL$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AM$3:AM$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AN$3:AN$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AO$3:AO$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AP$3:AP$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AQ$3:AQ$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AR$3:AR$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U21" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B21,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B21,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B21,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B21,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B21,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B21,'Raw Match Data'!AS$3:AS$128))/(3*$C21)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B22)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B22)</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!$AA$3:$AA$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AC$3:AC$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AD$3:AD$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AE$3:AE$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AF$3:AF$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AG$3:AG$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AH$3:AH$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AI$3:AI$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AJ$3:AJ$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AK$3:AK$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AL$3:AL$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AM$3:AM$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AN$3:AN$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AO$3:AO$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AP$3:AP$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AQ$3:AQ$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AR$3:AR$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U22" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B22,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B22,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B22,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B22,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B22,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B22,'Raw Match Data'!AS$3:AS$128))/(3*$C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="C23" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B23)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B23)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!$AA$3:$AA$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AC$3:AC$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AD$3:AD$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AE$3:AE$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AF$3:AF$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AG$3:AG$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AH$3:AH$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AI$3:AI$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AJ$3:AJ$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AK$3:AK$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AL$3:AL$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AM$3:AM$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AN$3:AN$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AO$3:AO$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AP$3:AP$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AQ$3:AQ$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AR$3:AR$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U23" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B23,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B23,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B23,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B23,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B23,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B23,'Raw Match Data'!AS$3:AS$128))/(3*$C23)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="C24" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B24)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B24)</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!$AA$3:$AA$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AC$3:AC$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AD$3:AD$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AE$3:AE$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AF$3:AF$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AG$3:AG$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AH$3:AH$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AI$3:AI$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AJ$3:AJ$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AK$3:AK$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AL$3:AL$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AM$3:AM$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AN$3:AN$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AO$3:AO$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AP$3:AP$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AQ$3:AQ$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AR$3:AR$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U24" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B24,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B24,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B24,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B24,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B24,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B24,'Raw Match Data'!AS$3:AS$128))/(3*$C24)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="C25" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B25)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B25)</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!$AA$3:$AA$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AC$3:AC$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AD$3:AD$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AE$3:AE$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AF$3:AF$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AG$3:AG$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AH$3:AH$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AI$3:AI$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AJ$3:AJ$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AK$3:AK$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AL$3:AL$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AM$3:AM$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AN$3:AN$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AO$3:AO$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AP$3:AP$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AQ$3:AQ$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AR$3:AR$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U25" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B25,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B25,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B25,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B25,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B25,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B25,'Raw Match Data'!AS$3:AS$128))/(3*$C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="C26" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B26)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B26)</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!$AA$3:$AA$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AC$3:AC$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AD$3:AD$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AE$3:AE$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AF$3:AF$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AG$3:AG$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AH$3:AH$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AI$3:AI$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AJ$3:AJ$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AK$3:AK$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AL$3:AL$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AM$3:AM$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AN$3:AN$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AO$3:AO$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AP$3:AP$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AQ$3:AQ$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AR$3:AR$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U26" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B26,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B26,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B26,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B26,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B26,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B26,'Raw Match Data'!AS$3:AS$128))/(3*$C26)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="C27" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B27)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B27)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!$AA$3:$AA$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AC$3:AC$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AD$3:AD$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AE$3:AE$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AF$3:AF$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AG$3:AG$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AH$3:AH$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AI$3:AI$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AJ$3:AJ$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AK$3:AK$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AL$3:AL$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AM$3:AM$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AN$3:AN$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AO$3:AO$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AP$3:AP$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AQ$3:AQ$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AR$3:AR$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U27" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B27,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B27,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B27,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B27,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B27,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B27,'Raw Match Data'!AS$3:AS$128))/(3*$C27)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="C28" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B28)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B28)</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!$AA$3:$AA$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AC$3:AC$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AD$3:AD$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AE$3:AE$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AF$3:AF$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AG$3:AG$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AH$3:AH$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AI$3:AI$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AJ$3:AJ$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AK$3:AK$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AL$3:AL$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AM$3:AM$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AN$3:AN$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AO$3:AO$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AP$3:AP$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AQ$3:AQ$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AR$3:AR$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U28" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B28,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B28,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B28,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B28,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B28,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B28,'Raw Match Data'!AS$3:AS$128))/(3*$C28)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="C29" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B29)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B29)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!$AA$3:$AA$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AC$3:AC$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AD$3:AD$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AE$3:AE$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AF$3:AF$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AG$3:AG$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AH$3:AH$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AI$3:AI$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AJ$3:AJ$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AK$3:AK$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AL$3:AL$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AM$3:AM$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AN$3:AN$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AO$3:AO$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AP$3:AP$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AQ$3:AQ$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AR$3:AR$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U29" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B29,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B29,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B29,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B29,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B29,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B29,'Raw Match Data'!AS$3:AS$128))/(3*$C29)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="C30" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B30)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B30)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!$AA$3:$AA$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AC$3:AC$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AD$3:AD$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AE$3:AE$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AF$3:AF$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AG$3:AG$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AH$3:AH$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AI$3:AI$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AJ$3:AJ$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AK$3:AK$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AL$3:AL$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AM$3:AM$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AN$3:AN$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AO$3:AO$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AP$3:AP$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AQ$3:AQ$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AR$3:AR$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U30" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B30,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B30,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B30,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B30,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B30,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B30,'Raw Match Data'!AS$3:AS$128))/(3*$C30)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="C31" s="3">
-        <f>COUNTIF('Raw Match Data'!$B$3:$D$128,$B31)+COUNTIF('Raw Match Data'!$X$3:$Z$128,$B31)</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="4" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!$E$3:$E$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!$AA$3:$AA$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!$AA$3:$AA$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!G$3:G$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AC$3:AC$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AC$3:AC$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!H$3:H$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AD$3:AD$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AD$3:AD$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!I$3:I$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AE$3:AE$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AE$3:AE$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!J$3:J$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AF$3:AF$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AF$3:AF$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!K$3:K$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AG$3:AG$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AG$3:AG$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!L$3:L$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AH$3:AH$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AH$3:AH$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!M$3:M$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AI$3:AI$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AI$3:AI$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!N$3:N$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AJ$3:AJ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AJ$3:AJ$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!O$3:O$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AK$3:AK$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AK$3:AK$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!P$3:P$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AL$3:AL$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AL$3:AL$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!Q$3:Q$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AM$3:AM$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AM$3:AM$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!R$3:R$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AN$3:AN$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AN$3:AN$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!S$3:S$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AO$3:AO$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AO$3:AO$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!T$3:T$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AP$3:AP$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AP$3:AP$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!U$3:U$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AQ$3:AQ$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AQ$3:AQ$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!V$3:V$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AR$3:AR$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AR$3:AR$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U31" s="5" t="e">
-        <f>SUM(SUMIF('Raw Match Data'!$B$3:$B$128,$B31,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$C$3:$C$128,$B31,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$D$3:$D$128,$B31,'Raw Match Data'!W$3:W$128),SUMIF('Raw Match Data'!$X$3:$X$128,$B31,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Y$3:$Y$128,$B31,'Raw Match Data'!AS$3:AS$128),SUMIF('Raw Match Data'!$Z$3:$Z$128,$B31,'Raw Match Data'!AS$3:AS$128))/(3*$C31)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C16" s="3"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C18" s="3"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C24" s="3"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C26" s="3"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C31" s="3"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>